<commit_message>
T3- Draft excel liste accès
</commit_message>
<xml_diff>
--- a/Travail 3/Création des listes d'accès.xlsx
+++ b/Travail 3/Création des listes d'accès.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="117">
   <si>
     <t>Interface</t>
   </si>
@@ -269,13 +269,115 @@
   </si>
   <si>
     <t>R_SS</t>
+  </si>
+  <si>
+    <t>192.168.60.0 /24</t>
+  </si>
+  <si>
+    <t>Requête aux serveurs et réponse vers le proprio</t>
+  </si>
+  <si>
+    <t>192.168.20.0 /24</t>
+  </si>
+  <si>
+    <t>Requête aux ordinateurs des administrateurs et réponse vers le proprio</t>
+  </si>
+  <si>
+    <t>192.168.30.0 /24</t>
+  </si>
+  <si>
+    <t>192.168.40.0 /24</t>
+  </si>
+  <si>
+    <t>192.168.50.0 /24</t>
+  </si>
+  <si>
+    <t>Requête aux ordinateurs des employés de production et réponse vers le proprio</t>
+  </si>
+  <si>
+    <t>Requête aux ordinateurs des employés R&amp;D et réponse vers le proprio</t>
+  </si>
+  <si>
+    <t>Requête aux ordinateurs des informaticiens et réponse vers le proprio</t>
+  </si>
+  <si>
+    <t>SMTP</t>
+  </si>
+  <si>
+    <t>Requête et réponse pour le serveur de courriel SMTP</t>
+  </si>
+  <si>
+    <t>POP3</t>
+  </si>
+  <si>
+    <t>Requête et réponse pour le serveur de courriel POP3</t>
+  </si>
+  <si>
+    <t>Requête et réponse du serveur DNS</t>
+  </si>
+  <si>
+    <t>fa0/0.2</t>
+  </si>
+  <si>
+    <t>Administrateurs</t>
+  </si>
+  <si>
+    <t>HTTP</t>
+  </si>
+  <si>
+    <t>192.168.60.20</t>
+  </si>
+  <si>
+    <t>192.168.60.10</t>
+  </si>
+  <si>
+    <t>192.168.60.30</t>
+  </si>
+  <si>
+    <t>fa0/0.3</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>192.168.60.40</t>
+  </si>
+  <si>
+    <t>Requête et réponse du serveur de production (site web)</t>
+  </si>
+  <si>
+    <t>Requête et réponse vers le serveur web Admin (site web)</t>
+  </si>
+  <si>
+    <t>fa0/0.4</t>
+  </si>
+  <si>
+    <t>Rech. &amp;  Dev.</t>
+  </si>
+  <si>
+    <t>192.168.60.50</t>
+  </si>
+  <si>
+    <t>Requête et réponse vers le serveur R&amp;D</t>
+  </si>
+  <si>
+    <t>fa0/0.5</t>
+  </si>
+  <si>
+    <t>Informaticiens</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Oui</t>
+  </si>
+  <si>
+    <t>Requête et réponse vers tous les serveurs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,6 +397,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -332,7 +442,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -402,11 +512,156 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -429,6 +684,60 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -438,31 +747,70 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -745,76 +1093,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="12" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="12" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="12" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" style="12" customWidth="1"/>
-    <col min="13" max="13" width="6" style="12" customWidth="1"/>
-    <col min="14" max="14" width="8.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="52" style="12" customWidth="1"/>
-    <col min="16" max="16" width="5.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.85546875" style="12"/>
+    <col min="1" max="1" width="10.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="5" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="9" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="9" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" style="9" customWidth="1"/>
+    <col min="13" max="13" width="6" style="9" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="78.28515625" style="9" customWidth="1"/>
+    <col min="16" max="16" width="5.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="5"/>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="7" t="s">
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
     </row>
     <row r="2" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="27"/>
+      <c r="G2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="10" t="s">
+      <c r="H2" s="27"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10" t="s">
+      <c r="K2" s="7"/>
+      <c r="L2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
     </row>
     <row r="3" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -829,34 +1177,34 @@
       <c r="D3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="7" t="s">
         <v>24</v>
       </c>
       <c r="O3" s="3" t="s">
@@ -867,1127 +1215,2194 @@
       </c>
     </row>
     <row r="4" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="N4" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="P4" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="14" t="s">
+      <c r="F6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="11">
         <v>53</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14" t="s">
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="P6" s="15">
+      <c r="P6" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17" t="s">
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="K7" s="17">
+      <c r="K7" s="14">
         <v>53</v>
       </c>
-      <c r="L7" s="17" t="s">
+      <c r="L7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="M7" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="N7" s="17" t="s">
+      <c r="M7" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="O7" s="17" t="s">
+      <c r="O7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="P7" s="18"/>
+      <c r="P7" s="15"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14" t="s">
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="L8" s="14" t="s">
+      <c r="K8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="M8" s="14">
+      <c r="M8" s="11">
         <v>80</v>
       </c>
-      <c r="N8" s="14" t="s">
+      <c r="N8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="O8" s="14"/>
-      <c r="P8" s="15">
+      <c r="O8" s="11"/>
+      <c r="P8" s="12">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="14">
         <v>80</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="17" t="s">
+      <c r="H9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="18"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="15"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="L10" s="12" t="s">
+      <c r="K10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="M10" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="N10" s="12" t="s">
+      <c r="M10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="P10" s="12">
+      <c r="P10" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="12" t="s">
+      <c r="F11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="12" t="s">
+      <c r="H11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="14" t="s">
+      <c r="F12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="11">
         <v>53</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14" t="s">
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="P12" s="15">
+      <c r="P12" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17" t="s">
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="17">
+      <c r="K13" s="14">
         <v>53</v>
       </c>
-      <c r="L13" s="17" t="s">
+      <c r="L13" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="M13" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="N13" s="17" t="s">
+      <c r="M13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="O13" s="17" t="s">
+      <c r="O13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="P13" s="18"/>
+      <c r="P13" s="15"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="14" t="s">
+      <c r="F14" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="11">
         <v>80</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14" t="s">
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="P14" s="15">
+      <c r="P14" s="12">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17" t="s">
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="17">
+      <c r="K15" s="14">
         <v>80</v>
       </c>
-      <c r="L15" s="17" t="s">
+      <c r="L15" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="M15" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="N15" s="17" t="s">
+      <c r="M15" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="N15" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="O15" s="17" t="s">
+      <c r="O15" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="P15" s="18"/>
+      <c r="P15" s="15"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="14" t="s">
+      <c r="F16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="11">
         <v>53</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="I16" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14" t="s">
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="P16" s="15">
+      <c r="P16" s="12">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17" t="s">
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="K17" s="17">
+      <c r="K17" s="14">
         <v>53</v>
       </c>
-      <c r="L17" s="17" t="s">
+      <c r="L17" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="M17" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="N17" s="17" t="s">
+      <c r="M17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="N17" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="O17" s="17" t="s">
+      <c r="O17" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="P17" s="18"/>
+      <c r="P17" s="15"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="14" t="s">
+      <c r="F18" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I18" s="14" t="s">
+      <c r="H18" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14" t="s">
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="P18" s="15">
+      <c r="P18" s="12">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17" t="s">
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="K19" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="L19" s="17" t="s">
+      <c r="K19" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="L19" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="N19" s="17" t="s">
+      <c r="M19" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="N19" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="O19" s="17" t="s">
+      <c r="O19" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="P19" s="18"/>
+      <c r="P19" s="15"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G20" s="14" t="s">
+      <c r="F20" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H20" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I20" s="14" t="s">
+      <c r="H20" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14" t="s">
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="P20" s="15">
+      <c r="P20" s="12">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17" t="s">
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="K21" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="L21" s="17" t="s">
+      <c r="K21" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="L21" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="M21" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="N21" s="17" t="s">
+      <c r="M21" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="N21" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="O21" s="17" t="s">
+      <c r="O21" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="P21" s="18"/>
+      <c r="P21" s="15"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G22" s="14" t="s">
+      <c r="F22" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H22" s="14">
+      <c r="H22" s="11">
         <v>53</v>
       </c>
-      <c r="I22" s="14" t="s">
+      <c r="I22" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14" t="s">
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="P22" s="15">
+      <c r="P22" s="12">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17" t="s">
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="K23" s="17">
+      <c r="K23" s="14">
         <v>53</v>
       </c>
-      <c r="L23" s="17" t="s">
+      <c r="L23" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="N23" s="17" t="s">
+      <c r="M23" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="N23" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="O23" s="17" t="s">
+      <c r="O23" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="P23" s="18"/>
+      <c r="P23" s="15"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" s="14" t="s">
+      <c r="F24" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="14">
+      <c r="H24" s="11">
         <v>80</v>
       </c>
-      <c r="I24" s="14" t="s">
+      <c r="I24" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14" t="s">
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="P24" s="15">
+      <c r="P24" s="12">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17" t="s">
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="K25" s="17">
+      <c r="K25" s="14">
         <v>80</v>
       </c>
-      <c r="L25" s="17" t="s">
+      <c r="L25" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="M25" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="N25" s="17" t="s">
+      <c r="M25" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="N25" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="O25" s="17" t="s">
+      <c r="O25" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="P25" s="18"/>
+      <c r="P25" s="15"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J26" s="12" t="s">
+      <c r="J26" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="K26" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="L26" s="12" t="s">
+      <c r="K26" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L26" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="M26" s="12">
+      <c r="M26" s="9">
         <v>53</v>
       </c>
-      <c r="N26" s="12" t="s">
+      <c r="N26" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="P26" s="12">
+      <c r="P26" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27" s="9">
         <v>53</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="G27" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H27" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I27" s="12" t="s">
+      <c r="H27" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J28" s="12" t="s">
+      <c r="J28" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K28" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="L28" s="12" t="s">
+      <c r="K28" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L28" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="M28" s="12">
+      <c r="M28" s="9">
         <v>53</v>
       </c>
-      <c r="N28" s="12" t="s">
+      <c r="N28" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="P28" s="12">
+      <c r="P28" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="12">
+      <c r="F29" s="9">
         <v>53</v>
       </c>
-      <c r="G29" s="12" t="s">
+      <c r="G29" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H29" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I29" s="12" t="s">
+      <c r="H29" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I29" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J30" s="12" t="s">
+      <c r="J30" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K30" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="L30" s="12" t="s">
+      <c r="K30" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L30" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="M30" s="12">
+      <c r="M30" s="9">
         <v>53</v>
       </c>
-      <c r="N30" s="12" t="s">
+      <c r="N30" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="P30" s="12">
+      <c r="P30" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="12">
+      <c r="F31" s="9">
         <v>53</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="G31" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H31" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I31" s="12" t="s">
+      <c r="H31" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I31" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J32" s="12" t="s">
+      <c r="J32" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K32" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="L32" s="12" t="s">
+      <c r="K32" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L32" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="M32" s="12">
+      <c r="M32" s="9">
         <v>53</v>
       </c>
-      <c r="N32" s="12" t="s">
+      <c r="N32" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="P32" s="12">
+      <c r="P32" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F33" s="12">
+      <c r="F33" s="9">
         <v>53</v>
       </c>
-      <c r="G33" s="12" t="s">
+      <c r="G33" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H33" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I33" s="12" t="s">
+      <c r="H33" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I33" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="J34" s="12" t="s">
+      <c r="J34" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K34" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="L34" s="12" t="s">
+      <c r="K34" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="M34" s="12">
+      <c r="M34" s="9">
         <v>80</v>
       </c>
-      <c r="N34" s="12" t="s">
+      <c r="N34" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="P34" s="12">
+      <c r="P34" s="9">
         <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F35" s="12">
+      <c r="F35" s="9">
         <v>80</v>
       </c>
-      <c r="G35" s="12" t="s">
+      <c r="G35" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H35" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I35" s="12" t="s">
+      <c r="H35" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I35" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="J36" s="12" t="s">
+      <c r="J36" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K36" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="L36" s="12" t="s">
+      <c r="K36" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L36" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="M36" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="N36" s="12" t="s">
+      <c r="M36" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="N36" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="P36" s="12">
+      <c r="P36" s="9">
         <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E37" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F37" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G37" s="12" t="s">
+      <c r="F37" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H37" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I37" s="12" t="s">
+      <c r="H37" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I37" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
+    <row r="39" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="31" t="s">
         <v>82</v>
       </c>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="32"/>
+      <c r="L40" s="32"/>
+      <c r="M40" s="32"/>
+      <c r="N40" s="32"/>
+      <c r="O40" s="33"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="6" t="s">
+      <c r="A41" s="49"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="7" t="s">
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="7"/>
-      <c r="N41" s="7"/>
-      <c r="O41" s="3"/>
+      <c r="K41" s="38"/>
+      <c r="L41" s="38"/>
+      <c r="M41" s="38"/>
+      <c r="N41" s="38"/>
+      <c r="O41" s="50"/>
       <c r="P41" s="3"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="8" t="s">
+      <c r="A42" s="49"/>
+      <c r="B42" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="6" t="s">
+      <c r="C42" s="43"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6" t="s">
+      <c r="F42" s="37"/>
+      <c r="G42" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="H42" s="6"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="10" t="s">
+      <c r="H42" s="37"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="K42" s="10"/>
-      <c r="L42" s="10" t="s">
+      <c r="K42" s="40"/>
+      <c r="L42" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="M42" s="10"/>
-      <c r="N42" s="10"/>
-      <c r="O42" s="3"/>
+      <c r="M42" s="40"/>
+      <c r="N42" s="40"/>
+      <c r="O42" s="50"/>
       <c r="P42" s="3"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E43" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="F43" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="G43" s="9" t="s">
+      <c r="G43" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="H43" s="9" t="s">
+      <c r="H43" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="I43" s="9" t="s">
+      <c r="I43" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="J43" s="10" t="s">
+      <c r="J43" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="K43" s="10" t="s">
+      <c r="K43" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="L43" s="10" t="s">
+      <c r="L43" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="M43" s="10" t="s">
+      <c r="M43" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N43" s="10" t="s">
+      <c r="N43" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="O43" s="3" t="s">
+      <c r="O43" s="48" t="s">
         <v>18</v>
       </c>
       <c r="P43" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
+    <row r="44" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="11" t="s">
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="F44" s="11" t="s">
+      <c r="F44" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="G44" s="11" t="s">
+      <c r="G44" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="H44" s="11" t="s">
+      <c r="H44" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="I44" s="11" t="s">
+      <c r="I44" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="J44" s="11" t="s">
+      <c r="J44" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="K44" s="11" t="s">
+      <c r="K44" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="L44" s="11" t="s">
+      <c r="L44" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="M44" s="11" t="s">
+      <c r="M44" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="N44" s="11" t="s">
+      <c r="N44" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="O44" s="5"/>
-      <c r="P44" s="11" t="s">
+      <c r="O44" s="36"/>
+      <c r="P44" s="8" t="s">
         <v>74</v>
       </c>
     </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F45" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G45" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="H45" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I45" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J45" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="K45" s="29"/>
+      <c r="L45" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="M45" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N45" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O45" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="P45" s="19">
+        <v>1</v>
+      </c>
+    </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B46" s="12" t="s">
+      <c r="A46" s="20"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="C46" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D46" s="12" t="s">
+      <c r="F46" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G46" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="H46" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I46" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J46" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="K46" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="L46" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="M46" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N46" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O46" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="P46" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="20"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E47" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="F46" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G46" s="12" t="s">
+      <c r="F47" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G47" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="H47" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I47" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J47" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="K47" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="L47" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="M47" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N47" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O47" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="P47" s="22"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="20"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F48" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G48" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="H48" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I48" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J48" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="K48" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="L48" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="M48" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N48" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O48" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="P48" s="22"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="20"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F49" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G49" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="H49" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I49" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J49" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="K49" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="L49" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="M49" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N49" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O49" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="P49" s="22"/>
+    </row>
+    <row r="50" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="23"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E50" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="F50" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G50" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="H50" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="I50" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="J50" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="K50" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="L50" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="M50" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="N50" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="O50" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="P50" s="25"/>
+    </row>
+    <row r="51" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="20"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="21"/>
+      <c r="M51" s="21"/>
+      <c r="N51" s="21"/>
+      <c r="O51" s="22"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D52" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E52" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F52" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G52" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="H46" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I46" s="12" t="s">
+      <c r="H52" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I52" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="J46" s="12" t="s">
+      <c r="J52" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="K46" s="19"/>
-      <c r="L46" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="M46" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="N46" s="12" t="s">
+      <c r="K52" s="18"/>
+      <c r="L52" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="M52" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="N52" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="O46" s="12" t="s">
+      <c r="O52" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="P46" s="12">
-        <v>1</v>
+      <c r="P52" s="19"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" s="20"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G53" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="H53" s="21">
+        <v>80</v>
+      </c>
+      <c r="I53" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J53" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="K53" s="21">
+        <v>80</v>
+      </c>
+      <c r="L53" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="M53" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N53" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O53" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="P53" s="22"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" s="20"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E54" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G54" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="H54" s="21">
+        <v>53</v>
+      </c>
+      <c r="I54" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J54" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="K54" s="21">
+        <v>53</v>
+      </c>
+      <c r="L54" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="M54" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N54" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O54" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="P54" s="22"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" s="20"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E55" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F55" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G55" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="H55" s="21">
+        <v>25</v>
+      </c>
+      <c r="I55" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J55" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="K55" s="21">
+        <v>25</v>
+      </c>
+      <c r="L55" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="M55" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N55" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O55" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="P55" s="22"/>
+    </row>
+    <row r="56" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="23"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="E56" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="F56" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G56" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="H56" s="24">
+        <v>110</v>
+      </c>
+      <c r="I56" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="J56" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="K56" s="24">
+        <v>110</v>
+      </c>
+      <c r="L56" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="M56" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="N56" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="O56" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="P56" s="25"/>
+    </row>
+    <row r="57" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="20"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
+      <c r="H57" s="21"/>
+      <c r="I57" s="21"/>
+      <c r="J57" s="21"/>
+      <c r="K57" s="21"/>
+      <c r="L57" s="21"/>
+      <c r="M57" s="21"/>
+      <c r="N57" s="21"/>
+      <c r="O57" s="22"/>
+      <c r="P57" s="21"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E58" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F58" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G58" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="H58" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I58" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="J58" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="K58" s="17"/>
+      <c r="L58" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="M58" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="N58" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="O58" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="P58" s="21"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" s="20"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G59" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="H59" s="21">
+        <v>25</v>
+      </c>
+      <c r="I59" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J59" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="K59" s="21">
+        <v>25</v>
+      </c>
+      <c r="L59" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="M59" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N59" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O59" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="P59" s="21"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" s="20"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F60" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G60" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="H60" s="21">
+        <v>110</v>
+      </c>
+      <c r="I60" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J60" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="K60" s="21">
+        <v>110</v>
+      </c>
+      <c r="L60" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="M60" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N60" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O60" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="P60" s="21"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" s="20"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E61" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F61" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G61" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="H61" s="21">
+        <v>53</v>
+      </c>
+      <c r="I61" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J61" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="K61" s="21">
+        <v>53</v>
+      </c>
+      <c r="L61" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="M61" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N61" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O61" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="P61" s="21"/>
+    </row>
+    <row r="62" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="23"/>
+      <c r="B62" s="24"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E62" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="F62" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G62" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="H62" s="24">
+        <v>80</v>
+      </c>
+      <c r="I62" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="J62" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="K62" s="24">
+        <v>80</v>
+      </c>
+      <c r="L62" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="M62" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="N62" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="O62" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="P62" s="21"/>
+    </row>
+    <row r="63" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="20"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="21"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="21"/>
+      <c r="J63" s="21"/>
+      <c r="K63" s="21"/>
+      <c r="L63" s="21"/>
+      <c r="M63" s="21"/>
+      <c r="N63" s="21"/>
+      <c r="O63" s="22"/>
+      <c r="P63" s="21"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E64" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="F64" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G64" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="H64" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I64" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="J64" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="K64" s="18"/>
+      <c r="L64" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="M64" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="N64" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="O64" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="P64" s="21"/>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A65" s="20"/>
+      <c r="B65" s="21"/>
+      <c r="C65" s="21"/>
+      <c r="D65" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E65" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F65" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G65" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="H65" s="21">
+        <v>25</v>
+      </c>
+      <c r="I65" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J65" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="K65" s="21">
+        <v>25</v>
+      </c>
+      <c r="L65" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="M65" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N65" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O65" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="P65" s="21"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66" s="20"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="E66" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F66" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G66" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="H66" s="21">
+        <v>110</v>
+      </c>
+      <c r="I66" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J66" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="K66" s="21">
+        <v>110</v>
+      </c>
+      <c r="L66" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="M66" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N66" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O66" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="P66" s="21"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A67" s="20"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E67" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F67" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G67" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="H67" s="21">
+        <v>53</v>
+      </c>
+      <c r="I67" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J67" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="K67" s="21">
+        <v>53</v>
+      </c>
+      <c r="L67" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="M67" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N67" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O67" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="P67" s="21"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" s="20"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E68" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F68" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G68" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="H68" s="21">
+        <v>80</v>
+      </c>
+      <c r="I68" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J68" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="K68" s="21">
+        <v>80</v>
+      </c>
+      <c r="L68" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="M68" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N68" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O68" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="P68" s="21"/>
+    </row>
+    <row r="69" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="23"/>
+      <c r="B69" s="24"/>
+      <c r="C69" s="24"/>
+      <c r="D69" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E69" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="F69" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G69" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="H69" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="I69" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="J69" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="K69" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="L69" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="M69" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="N69" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="O69" s="25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="20"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="21"/>
+      <c r="E70" s="21"/>
+      <c r="F70" s="21"/>
+      <c r="G70" s="21"/>
+      <c r="H70" s="21"/>
+      <c r="I70" s="21"/>
+      <c r="J70" s="21"/>
+      <c r="K70" s="21"/>
+      <c r="L70" s="21"/>
+      <c r="M70" s="21"/>
+      <c r="N70" s="21"/>
+      <c r="O70" s="22"/>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A71" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B71" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D71" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E71" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F71" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G71" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="H71" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I71" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="J71" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="K71" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="L71" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="M71" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="N71" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="O71" s="19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="23"/>
+      <c r="B72" s="24"/>
+      <c r="C72" s="24"/>
+      <c r="D72" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E72" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="F72" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G72" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="H72" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="I72" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="J72" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="K72" s="30"/>
+      <c r="L72" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="M72" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="N72" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="O72" s="25" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A40:O40"/>
     <mergeCell ref="E41:I41"/>
     <mergeCell ref="J41:N41"/>
     <mergeCell ref="B42:C42"/>

</xml_diff>